<commit_message>
added GNS and GUSB
</commit_message>
<xml_diff>
--- a/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
+++ b/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="310">
   <si>
     <t>Gene</t>
   </si>
@@ -949,9 +949,6 @@
   </si>
   <si>
     <t xml:space="preserve">*note: this one had 38 mutations but they seem to be wrong </t>
-  </si>
-  <si>
-    <t>2.6965E+308</t>
   </si>
 </sst>
 </file>
@@ -1200,9 +1197,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="346">
+  <cellStyleXfs count="356">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1633,7 +1640,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="346">
+  <cellStyles count="356">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1806,6 +1813,11 @@
     <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1978,6 +1990,11 @@
     <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2311,7 +2328,7 @@
   <dimension ref="A1:AG262"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116:AG116"/>
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13705,8 +13722,8 @@
       <c r="C116" s="37">
         <v>0.80154400000000003</v>
       </c>
-      <c r="D116" s="73" t="s">
-        <v>310</v>
+      <c r="D116" s="82" t="s">
+        <v>33</v>
       </c>
       <c r="E116" s="37">
         <v>0.64883363900000002</v>
@@ -13714,8 +13731,8 @@
       <c r="F116" s="37">
         <v>0.77370799999999995</v>
       </c>
-      <c r="G116" s="73" t="s">
-        <v>310</v>
+      <c r="G116" s="82" t="s">
+        <v>33</v>
       </c>
       <c r="H116" s="37">
         <v>3.3510703610000001</v>
@@ -13723,8 +13740,8 @@
       <c r="I116" s="37">
         <v>4.5971760000000002</v>
       </c>
-      <c r="J116" s="73" t="s">
-        <v>310</v>
+      <c r="J116" s="82" t="s">
+        <v>33</v>
       </c>
       <c r="K116" s="37">
         <v>5</v>
@@ -13795,9 +13812,103 @@
       <c r="AG116" s="37"/>
     </row>
     <row r="117" spans="1:33">
-      <c r="A117" t="s">
+      <c r="A117" s="37" t="s">
         <v>156</v>
       </c>
+      <c r="B117" s="37">
+        <v>0.72959668499999997</v>
+      </c>
+      <c r="C117" s="37">
+        <v>0.80373000000000006</v>
+      </c>
+      <c r="D117" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="E117" s="37">
+        <v>0.61217288000000003</v>
+      </c>
+      <c r="F117" s="37">
+        <v>0.77825</v>
+      </c>
+      <c r="G117" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="H117" s="37">
+        <v>3.046977101</v>
+      </c>
+      <c r="I117" s="37">
+        <v>3.9909349999999999</v>
+      </c>
+      <c r="J117" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="K117" s="37">
+        <v>2</v>
+      </c>
+      <c r="L117" s="37">
+        <v>0</v>
+      </c>
+      <c r="M117" s="38">
+        <v>0</v>
+      </c>
+      <c r="N117" s="37">
+        <v>1</v>
+      </c>
+      <c r="O117" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="P117" s="38">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="Q117" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="R117" s="37">
+        <v>0.109386293</v>
+      </c>
+      <c r="S117" s="37">
+        <v>9.6100000000000005E-3</v>
+      </c>
+      <c r="T117" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="U117" s="37">
+        <v>0.23279208900000001</v>
+      </c>
+      <c r="V117" s="37">
+        <v>0.15106</v>
+      </c>
+      <c r="W117" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="X117" s="37">
+        <v>1.853748602</v>
+      </c>
+      <c r="Y117" s="37">
+        <v>0.79342500000000005</v>
+      </c>
+      <c r="Z117" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA117" s="40">
+        <v>3.5224235999999999E-2</v>
+      </c>
+      <c r="AB117" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC117" s="39">
+        <v>0.18255339600000001</v>
+      </c>
+      <c r="AD117" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE117" s="39">
+        <v>0.17206608200000001</v>
+      </c>
+      <c r="AF117" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG117" s="37"/>
     </row>
     <row r="118" spans="1:33">
       <c r="A118" t="s">

</xml_diff>

<commit_message>
added HYAL1 and IDS
</commit_message>
<xml_diff>
--- a/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
+++ b/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="311">
   <si>
     <t>Gene</t>
   </si>
@@ -949,6 +949,9 @@
   </si>
   <si>
     <t xml:space="preserve">*note: this one had 38 mutations but they seem to be wrong </t>
+  </si>
+  <si>
+    <t>2.6965E+308</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1200,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="392">
+  <cellStyleXfs count="400">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1590,8 +1593,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1662,7 +1673,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1677,7 +1687,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="392">
+  <cellStyles count="400">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1873,6 +1883,10 @@
     <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2068,6 +2082,10 @@
     <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2401,7 +2419,7 @@
   <dimension ref="A1:AG262"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+      <selection activeCell="A124" sqref="A124:AG124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9124,7 +9142,7 @@
       <c r="AE68" s="39">
         <v>5.6692465999999997E-2</v>
       </c>
-      <c r="AF68" s="71">
+      <c r="AF68" s="70">
         <v>7.6084450000000001E-3</v>
       </c>
       <c r="AG68" s="60"/>
@@ -9720,7 +9738,7 @@
       <c r="AF74" s="39">
         <v>0.104850603</v>
       </c>
-      <c r="AG74" s="74"/>
+      <c r="AG74" s="73"/>
     </row>
     <row r="75" spans="1:33">
       <c r="A75" s="37" t="s">
@@ -9819,13 +9837,13 @@
       <c r="AF75" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AG75" s="72"/>
+      <c r="AG75" s="71"/>
     </row>
     <row r="76" spans="1:33">
       <c r="A76" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B76" s="75">
+      <c r="B76" s="74">
         <v>0.65758644736842098</v>
       </c>
       <c r="C76" s="44">
@@ -9865,10 +9883,10 @@
       <c r="N76" s="43">
         <v>0</v>
       </c>
-      <c r="O76" s="76">
-        <v>0</v>
-      </c>
-      <c r="P76" s="76">
+      <c r="O76" s="75">
+        <v>0</v>
+      </c>
+      <c r="P76" s="75">
         <v>0</v>
       </c>
       <c r="Q76" s="67" t="s">
@@ -10146,7 +10164,7 @@
       <c r="I79" s="37">
         <v>2.5824500000000001</v>
       </c>
-      <c r="J79" s="73" t="s">
+      <c r="J79" s="72" t="s">
         <v>33</v>
       </c>
       <c r="K79" s="37">
@@ -10316,13 +10334,13 @@
       <c r="AF80" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AG80" s="72"/>
+      <c r="AG80" s="71"/>
     </row>
     <row r="81" spans="1:33">
       <c r="A81" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="B81" s="75">
+      <c r="B81" s="74">
         <v>0.64893471471471442</v>
       </c>
       <c r="C81" s="43">
@@ -10334,7 +10352,7 @@
       <c r="E81" s="44">
         <v>0.51508828828828856</v>
       </c>
-      <c r="F81" s="77">
+      <c r="F81" s="76">
         <v>0.48420000000000002</v>
       </c>
       <c r="G81" s="43" t="s">
@@ -10343,7 +10361,7 @@
       <c r="H81" s="42">
         <v>2.1290223723723707</v>
       </c>
-      <c r="I81" s="77">
+      <c r="I81" s="76">
         <v>2.1036800000000002</v>
       </c>
       <c r="J81" s="43" t="s">
@@ -10362,16 +10380,16 @@
       <c r="N81" s="43">
         <v>0</v>
       </c>
-      <c r="O81" s="76">
-        <v>0</v>
-      </c>
-      <c r="P81" s="76">
+      <c r="O81" s="75">
+        <v>0</v>
+      </c>
+      <c r="P81" s="75">
         <v>0</v>
       </c>
       <c r="Q81" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="R81" s="75">
+      <c r="R81" s="74">
         <v>0.13716750238059713</v>
       </c>
       <c r="S81" s="42">
@@ -10481,7 +10499,7 @@
       <c r="U82" s="37">
         <v>0.361897898</v>
       </c>
-      <c r="V82" s="73">
+      <c r="V82" s="72">
         <v>1.11022E-16</v>
       </c>
       <c r="W82" s="37">
@@ -10909,13 +10927,13 @@
       <c r="AF86" s="39">
         <v>0.333286007</v>
       </c>
-      <c r="AG86" s="72"/>
+      <c r="AG86" s="71"/>
     </row>
     <row r="87" spans="1:33">
       <c r="A87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B87" s="78">
+      <c r="B87" s="77">
         <v>0.64347245353159865</v>
       </c>
       <c r="C87" s="11">
@@ -11014,7 +11032,7 @@
       <c r="A88" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B88" s="78">
+      <c r="B88" s="77">
         <v>0.70090894607843091</v>
       </c>
       <c r="C88" s="3">
@@ -11122,19 +11140,19 @@
       <c r="D89" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E89" s="79">
+      <c r="E89" s="78">
         <v>0.59064257692307709</v>
       </c>
-      <c r="F89" s="77">
+      <c r="F89" s="76">
         <v>0.5711033333333333</v>
       </c>
       <c r="G89" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="H89" s="79">
+      <c r="H89" s="78">
         <v>2.2729964615384617</v>
       </c>
-      <c r="I89" s="77">
+      <c r="I89" s="76">
         <v>1.8472200000000001</v>
       </c>
       <c r="J89" s="43" t="s">
@@ -11189,19 +11207,19 @@
       <c r="Z89" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="AA89" s="77">
+      <c r="AA89" s="76">
         <v>0.1538948</v>
       </c>
       <c r="AB89" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="AC89" s="77">
+      <c r="AC89" s="76">
         <v>0.18041879999999999</v>
       </c>
       <c r="AD89" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="AE89" s="77">
+      <c r="AE89" s="76">
         <v>6.5507239999999994E-2</v>
       </c>
       <c r="AF89" s="43" t="s">
@@ -11605,7 +11623,7 @@
       <c r="AG93" s="37"/>
     </row>
     <row r="94" spans="1:33">
-      <c r="A94" s="80" t="s">
+      <c r="A94" s="79" t="s">
         <v>134</v>
       </c>
       <c r="B94" s="37">
@@ -12495,7 +12513,7 @@
       <c r="AF102" s="52">
         <v>6.1207164000000001E-2</v>
       </c>
-      <c r="AG102" s="72"/>
+      <c r="AG102" s="71"/>
     </row>
     <row r="103" spans="1:33">
       <c r="A103" s="37" t="s">
@@ -13389,7 +13407,7 @@
       <c r="AG111" s="37"/>
     </row>
     <row r="112" spans="1:33">
-      <c r="A112" s="80" t="s">
+      <c r="A112" s="79" t="s">
         <v>151</v>
       </c>
       <c r="B112" s="37">
@@ -13589,7 +13607,7 @@
       <c r="AG113" s="37"/>
     </row>
     <row r="114" spans="1:33">
-      <c r="A114" s="81" t="s">
+      <c r="A114" s="80" t="s">
         <v>153</v>
       </c>
       <c r="B114" s="50">
@@ -13598,7 +13616,7 @@
       <c r="C114" s="50">
         <v>0.77210999999999996</v>
       </c>
-      <c r="D114" s="82" t="s">
+      <c r="D114" s="81" t="s">
         <v>33</v>
       </c>
       <c r="E114" s="50">
@@ -13607,7 +13625,7 @@
       <c r="F114" s="50">
         <v>0.70910333299999995</v>
       </c>
-      <c r="G114" s="82" t="s">
+      <c r="G114" s="81" t="s">
         <v>33</v>
       </c>
       <c r="H114" s="50">
@@ -13616,7 +13634,7 @@
       <c r="I114" s="50">
         <v>2.5824500000000001</v>
       </c>
-      <c r="J114" s="82" t="s">
+      <c r="J114" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K114" s="50">
@@ -13795,7 +13813,7 @@
       <c r="C116" s="37">
         <v>0.80154400000000003</v>
       </c>
-      <c r="D116" s="82" t="s">
+      <c r="D116" s="81" t="s">
         <v>33</v>
       </c>
       <c r="E116" s="37">
@@ -13804,7 +13822,7 @@
       <c r="F116" s="37">
         <v>0.77370799999999995</v>
       </c>
-      <c r="G116" s="82" t="s">
+      <c r="G116" s="81" t="s">
         <v>33</v>
       </c>
       <c r="H116" s="37">
@@ -13813,7 +13831,7 @@
       <c r="I116" s="37">
         <v>4.5971760000000002</v>
       </c>
-      <c r="J116" s="82" t="s">
+      <c r="J116" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K116" s="37">
@@ -13894,7 +13912,7 @@
       <c r="C117" s="37">
         <v>0.80373000000000006</v>
       </c>
-      <c r="D117" s="73" t="s">
+      <c r="D117" s="72" t="s">
         <v>33</v>
       </c>
       <c r="E117" s="37">
@@ -13903,7 +13921,7 @@
       <c r="F117" s="37">
         <v>0.77825</v>
       </c>
-      <c r="G117" s="73" t="s">
+      <c r="G117" s="72" t="s">
         <v>33</v>
       </c>
       <c r="H117" s="37">
@@ -13912,7 +13930,7 @@
       <c r="I117" s="37">
         <v>3.9909349999999999</v>
       </c>
-      <c r="J117" s="73" t="s">
+      <c r="J117" s="72" t="s">
         <v>33</v>
       </c>
       <c r="K117" s="37">
@@ -14083,7 +14101,7 @@
       <c r="AG118" s="50"/>
     </row>
     <row r="119" spans="1:33" s="3" customFormat="1">
-      <c r="A119" s="83" t="s">
+      <c r="A119" s="82" t="s">
         <v>159</v>
       </c>
       <c r="B119" s="33">
@@ -14478,14 +14496,202 @@
       <c r="AG122" s="37"/>
     </row>
     <row r="123" spans="1:33">
-      <c r="A123" t="s">
+      <c r="A123" s="37" t="s">
         <v>163</v>
       </c>
+      <c r="B123" s="37">
+        <v>0.70684482800000004</v>
+      </c>
+      <c r="C123" s="37">
+        <v>0.76298999999999995</v>
+      </c>
+      <c r="D123" s="72" t="s">
+        <v>310</v>
+      </c>
+      <c r="E123" s="37">
+        <v>0.44406834499999998</v>
+      </c>
+      <c r="F123" s="37">
+        <v>0.71892999999999996</v>
+      </c>
+      <c r="G123" s="72" t="s">
+        <v>310</v>
+      </c>
+      <c r="H123" s="37">
+        <v>1.8091450570000001</v>
+      </c>
+      <c r="I123" s="37">
+        <v>3.8573300000000001</v>
+      </c>
+      <c r="J123" s="72" t="s">
+        <v>310</v>
+      </c>
+      <c r="K123" s="37">
+        <v>1</v>
+      </c>
+      <c r="L123" s="37">
+        <v>0</v>
+      </c>
+      <c r="M123" s="38">
+        <v>0</v>
+      </c>
+      <c r="N123" s="37">
+        <v>1</v>
+      </c>
+      <c r="O123" s="38">
+        <v>1</v>
+      </c>
+      <c r="P123" s="38">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="Q123" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="R123" s="37">
+        <v>6.2974477000000001E-2</v>
+      </c>
+      <c r="S123" s="37">
+        <v>0</v>
+      </c>
+      <c r="T123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="U123" s="37">
+        <v>0.19751079899999999</v>
+      </c>
+      <c r="V123" s="37">
+        <v>0</v>
+      </c>
+      <c r="W123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="X123" s="37">
+        <v>2.0620370590000001</v>
+      </c>
+      <c r="Y123" s="37">
+        <v>0</v>
+      </c>
+      <c r="Z123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF123" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG123" s="37"/>
     </row>
     <row r="124" spans="1:33">
-      <c r="A124" s="70" t="s">
+      <c r="A124" s="37" t="s">
         <v>164</v>
       </c>
+      <c r="B124" s="37">
+        <v>0.73022267299999999</v>
+      </c>
+      <c r="C124" s="37">
+        <v>0.769101111</v>
+      </c>
+      <c r="D124" s="37">
+        <v>0.67315999999999998</v>
+      </c>
+      <c r="E124" s="37">
+        <v>0.58864454499999996</v>
+      </c>
+      <c r="F124" s="37">
+        <v>0.733897778</v>
+      </c>
+      <c r="G124" s="37">
+        <v>0.36413000000000001</v>
+      </c>
+      <c r="H124" s="37">
+        <v>2.8676153270000002</v>
+      </c>
+      <c r="I124" s="37">
+        <v>4.0629566669999999</v>
+      </c>
+      <c r="J124" s="37">
+        <v>-1.1180300000000001</v>
+      </c>
+      <c r="K124" s="37">
+        <v>19</v>
+      </c>
+      <c r="L124" s="37">
+        <v>1</v>
+      </c>
+      <c r="M124" s="38">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="N124" s="37">
+        <v>12</v>
+      </c>
+      <c r="O124" s="38">
+        <v>0.63160000000000005</v>
+      </c>
+      <c r="P124" s="38">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="Q124" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="R124" s="37">
+        <v>9.8935541000000002E-2</v>
+      </c>
+      <c r="S124" s="37">
+        <v>0.10883071499999999</v>
+      </c>
+      <c r="T124" s="37">
+        <v>0</v>
+      </c>
+      <c r="U124" s="37">
+        <v>0.251617706</v>
+      </c>
+      <c r="V124" s="37">
+        <v>0.22503693</v>
+      </c>
+      <c r="W124" s="37">
+        <v>0</v>
+      </c>
+      <c r="X124" s="37">
+        <v>2.1084568520000002</v>
+      </c>
+      <c r="Y124" s="37">
+        <v>1.7992739019999999</v>
+      </c>
+      <c r="Z124" s="37">
+        <v>0</v>
+      </c>
+      <c r="AA124" s="39">
+        <v>7.6552931000000005E-2</v>
+      </c>
+      <c r="AB124" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC124" s="40">
+        <v>7.8432099999999998E-3</v>
+      </c>
+      <c r="AD124" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE124" s="40">
+        <v>6.7301009999999996E-3</v>
+      </c>
+      <c r="AF124" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG124" s="37"/>
     </row>
     <row r="125" spans="1:33">
       <c r="A125" s="49" t="s">

</xml_diff>

<commit_message>
added basic script to analyze screen data
</commit_message>
<xml_diff>
--- a/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
+++ b/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="311">
   <si>
     <t>Gene</t>
   </si>
@@ -1200,7 +1200,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="416">
+  <cellStyleXfs count="420">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1617,8 +1617,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1700,8 +1704,9 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="416">
+  <cellStyles count="420">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1909,6 +1914,8 @@
     <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2116,6 +2123,8 @@
     <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2449,7 +2458,7 @@
   <dimension ref="A1:AG262"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:AG127"/>
+      <selection activeCell="A129" sqref="A129:AG129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15021,86 +15030,274 @@
       <c r="AG127" s="34"/>
     </row>
     <row r="128" spans="1:33">
-      <c r="A128" t="s">
+      <c r="A128" s="34" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129" t="s">
+      <c r="B128" s="34">
+        <v>0.73189674400000004</v>
+      </c>
+      <c r="C128" s="34">
+        <v>0.79793199999999997</v>
+      </c>
+      <c r="D128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E128" s="34">
+        <v>0.642705843</v>
+      </c>
+      <c r="F128" s="34">
+        <v>0.83290299999999995</v>
+      </c>
+      <c r="G128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H128" s="34">
+        <v>3.2030907270000002</v>
+      </c>
+      <c r="I128" s="34">
+        <v>4.4197810000000004</v>
+      </c>
+      <c r="J128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K128" s="34">
+        <v>10</v>
+      </c>
+      <c r="L128" s="34">
+        <v>0</v>
+      </c>
+      <c r="M128" s="35">
+        <v>0</v>
+      </c>
+      <c r="N128" s="34">
+        <v>7</v>
+      </c>
+      <c r="O128" s="35">
+        <v>0.7</v>
+      </c>
+      <c r="P128" s="35">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="Q128" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="R128" s="34">
+        <v>0.10511651299999999</v>
+      </c>
+      <c r="S128" s="34">
+        <v>9.1529544000000004E-2</v>
+      </c>
+      <c r="T128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="U128" s="34">
+        <v>0.26104797000000002</v>
+      </c>
+      <c r="V128" s="34">
+        <v>0.27839491599999999</v>
+      </c>
+      <c r="W128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="X128" s="34">
+        <v>1.554072839</v>
+      </c>
+      <c r="Y128" s="34">
+        <v>1.47477244</v>
+      </c>
+      <c r="Z128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA128" s="37">
+        <v>2.4801729000000002E-2</v>
+      </c>
+      <c r="AB128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC128" s="37">
+        <v>2.9955017E-2</v>
+      </c>
+      <c r="AD128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE128" s="37">
+        <v>1.4488338999999999E-2</v>
+      </c>
+      <c r="AF128" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG128" s="34"/>
+    </row>
+    <row r="129" spans="1:33">
+      <c r="A129" s="34" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129" s="34">
+        <v>0.72571502600000004</v>
+      </c>
+      <c r="C129" s="43">
+        <v>0.76885000000000003</v>
+      </c>
+      <c r="D129" s="34">
+        <v>0.77344999999999997</v>
+      </c>
+      <c r="E129" s="34">
+        <v>0.58834505299999995</v>
+      </c>
+      <c r="F129" s="34">
+        <v>0.60326000000000002</v>
+      </c>
+      <c r="G129" s="34">
+        <v>0.44046000000000002</v>
+      </c>
+      <c r="H129" s="34">
+        <v>2.8661265340000002</v>
+      </c>
+      <c r="I129" s="34">
+        <v>3.357272</v>
+      </c>
+      <c r="J129" s="34">
+        <v>2.0487899999999999</v>
+      </c>
+      <c r="K129" s="34">
+        <v>6</v>
+      </c>
+      <c r="L129" s="34">
+        <v>1</v>
+      </c>
+      <c r="M129" s="35">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="N129" s="34">
+        <v>1</v>
+      </c>
+      <c r="O129" s="35">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="P129" s="35">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="Q129" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="R129" s="34">
+        <v>0.10064461700000001</v>
+      </c>
+      <c r="S129" s="34">
+        <v>5.0387545999999998E-2</v>
+      </c>
+      <c r="T129" s="34">
+        <v>0</v>
+      </c>
+      <c r="U129" s="34">
+        <v>0.203562565</v>
+      </c>
+      <c r="V129" s="34">
+        <v>0.13152716</v>
+      </c>
+      <c r="W129" s="34">
+        <v>0</v>
+      </c>
+      <c r="X129" s="34">
+        <v>1.5161377620000001</v>
+      </c>
+      <c r="Y129" s="34">
+        <v>1.831007077</v>
+      </c>
+      <c r="Z129" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA129" s="36">
+        <v>6.5916970000000005E-2</v>
+      </c>
+      <c r="AB129" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC129" s="36">
+        <v>0.40688074099999999</v>
+      </c>
+      <c r="AD129" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE129" s="36">
+        <v>0.290891599</v>
+      </c>
+      <c r="AF129" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG129" s="34"/>
+    </row>
+    <row r="130" spans="1:33">
       <c r="A130" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:33">
       <c r="A131" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:33">
       <c r="A132" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:33">
       <c r="A133" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:33">
       <c r="A134" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:33">
       <c r="A135" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
-      <c r="A136" t="s">
+    <row r="136" spans="1:33">
+      <c r="A136" s="81" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:33">
       <c r="A137" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:33">
       <c r="A138" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:33">
       <c r="A139" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:33">
       <c r="A140" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:33">
       <c r="A141" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:33">
       <c r="A142" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:33">
       <c r="A143" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:33">
       <c r="A144" t="s">
         <v>183</v>
       </c>

</xml_diff>

<commit_message>
added LFNG and LIPA
</commit_message>
<xml_diff>
--- a/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
+++ b/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="312">
   <si>
     <t>Gene</t>
   </si>
@@ -952,6 +952,9 @@
   </si>
   <si>
     <t>2.6965E+308</t>
+  </si>
+  <si>
+    <t>hmzdy</t>
   </si>
 </sst>
 </file>
@@ -1200,9 +1203,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="420">
+  <cellStyleXfs count="428">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1706,7 +1717,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="420">
+  <cellStyles count="428">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1916,6 +1927,10 @@
     <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2125,6 +2140,10 @@
     <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2458,7 +2477,7 @@
   <dimension ref="A1:AG262"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129:AG129"/>
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15228,9 +15247,103 @@
       <c r="AG129" s="34"/>
     </row>
     <row r="130" spans="1:33">
-      <c r="A130" t="s">
+      <c r="A130" s="34" t="s">
         <v>169</v>
       </c>
+      <c r="B130" s="34">
+        <v>0.64851349599999997</v>
+      </c>
+      <c r="C130" s="34">
+        <v>0.74857399999999996</v>
+      </c>
+      <c r="D130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E130" s="34">
+        <v>0.40296756099999997</v>
+      </c>
+      <c r="F130" s="34">
+        <v>0.68442800000000004</v>
+      </c>
+      <c r="G130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H130" s="34">
+        <v>1.203668293</v>
+      </c>
+      <c r="I130" s="34">
+        <v>3.6802139999999999</v>
+      </c>
+      <c r="J130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K130" s="34">
+        <v>5</v>
+      </c>
+      <c r="L130" s="34">
+        <v>0</v>
+      </c>
+      <c r="M130" s="35">
+        <v>0</v>
+      </c>
+      <c r="N130" s="34">
+        <v>3</v>
+      </c>
+      <c r="O130" s="35">
+        <v>0.6</v>
+      </c>
+      <c r="P130" s="35">
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="Q130" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="R130" s="34">
+        <v>7.9070056E-2</v>
+      </c>
+      <c r="S130" s="34">
+        <v>8.5931357999999999E-2</v>
+      </c>
+      <c r="T130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="U130" s="34">
+        <v>0.18361965399999999</v>
+      </c>
+      <c r="V130" s="34">
+        <v>0.238047333</v>
+      </c>
+      <c r="W130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="X130" s="34">
+        <v>1.6689872809999999</v>
+      </c>
+      <c r="Y130" s="34">
+        <v>1.2619925599999999</v>
+      </c>
+      <c r="Z130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA130" s="37">
+        <v>3.0188415999999999E-2</v>
+      </c>
+      <c r="AB130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC130" s="37">
+        <v>2.8865814E-2</v>
+      </c>
+      <c r="AD130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE130" s="37">
+        <v>6.0442639999999997E-3</v>
+      </c>
+      <c r="AF130" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG130" s="34"/>
     </row>
     <row r="131" spans="1:33">
       <c r="A131" t="s">

</xml_diff>

<commit_message>
finished dataset prelim data
</commit_message>
<xml_diff>
--- a/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
+++ b/yeast_replaceable_genes/sequences/all_other_mendelian/mendelian_conservation_summary.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="314">
   <si>
     <t>Gene</t>
   </si>
@@ -956,17 +956,23 @@
     <t>hmzdy</t>
   </si>
   <si>
-    <t>2.6965E+308</t>
-  </si>
-  <si>
     <t>SDHA</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Divergence</t>
+  </si>
+  <si>
+    <t>overall p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1149,6 +1155,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -2150,7 +2163,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2291,6 +2304,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="854">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3483,11 +3500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH261"/>
+  <dimension ref="A1:AH264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A261" sqref="A261"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA264" sqref="AA264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -20908,7 +20925,7 @@
         <v>0.56920000000000004</v>
       </c>
       <c r="D177" s="109" t="s">
-        <v>310</v>
+        <v>33</v>
       </c>
       <c r="E177" s="78">
         <v>0.59275145799999995</v>
@@ -21795,7 +21812,7 @@
         <v>0.75850181800000005</v>
       </c>
       <c r="D186" s="109" t="s">
-        <v>310</v>
+        <v>33</v>
       </c>
       <c r="E186" s="78">
         <v>0.52575105300000002</v>
@@ -21804,7 +21821,7 @@
         <v>0.64782545499999999</v>
       </c>
       <c r="G186" s="109" t="s">
-        <v>310</v>
+        <v>33</v>
       </c>
       <c r="H186" s="78">
         <v>1.9987537150000001</v>
@@ -21813,7 +21830,7 @@
         <v>3.4460981820000001</v>
       </c>
       <c r="J186" s="109" t="s">
-        <v>310</v>
+        <v>33</v>
       </c>
       <c r="K186" s="78">
         <v>11</v>
@@ -24737,7 +24754,7 @@
     </row>
     <row r="216" spans="1:34">
       <c r="A216" s="78" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B216" s="78">
         <v>0.75491763599999995</v>
@@ -28052,22 +28069,22 @@
       <c r="Z249" s="77">
         <v>0.84249389500000005</v>
       </c>
-      <c r="AA249" s="77">
+      <c r="AA249" s="140">
         <v>3.0607600000000002E-4</v>
       </c>
-      <c r="AB249" s="77">
+      <c r="AB249" s="140">
         <v>3.4740367000000001E-2</v>
       </c>
-      <c r="AC249" s="77">
+      <c r="AC249" s="140">
         <v>4.4074689999999998E-3</v>
       </c>
-      <c r="AD249" s="77">
+      <c r="AD249" s="140">
         <v>8.2173939999999994E-3</v>
       </c>
-      <c r="AE249" s="77">
+      <c r="AE249" s="140">
         <v>1.0876900000000001E-3</v>
       </c>
-      <c r="AF249" s="77">
+      <c r="AF249" s="140">
         <v>1.6749351999999999E-2</v>
       </c>
     </row>
@@ -28150,22 +28167,22 @@
       <c r="Z250" s="77">
         <v>1.6421448329999999</v>
       </c>
-      <c r="AA250" s="77">
+      <c r="AA250" s="140">
         <v>3.6394013000000003E-2</v>
       </c>
-      <c r="AB250" s="77">
+      <c r="AB250" s="141">
         <v>5.6547782999999997E-2</v>
       </c>
-      <c r="AC250" s="77">
+      <c r="AC250" s="141">
         <v>0.12783530400000001</v>
       </c>
-      <c r="AD250" s="77">
+      <c r="AD250" s="140">
         <v>2.1004726000000001E-2</v>
       </c>
-      <c r="AE250" s="77">
+      <c r="AE250" s="141">
         <v>0.265244759</v>
       </c>
-      <c r="AF250" s="77">
+      <c r="AF250" s="140">
         <v>1.6045802000000001E-2</v>
       </c>
     </row>
@@ -28346,22 +28363,22 @@
       <c r="Z252" s="77">
         <v>0.34010499999999999</v>
       </c>
-      <c r="AA252" s="77">
+      <c r="AA252" s="141">
         <v>0.196909641</v>
       </c>
-      <c r="AB252" s="77">
+      <c r="AB252" s="141">
         <v>0.20993869100000001</v>
       </c>
-      <c r="AC252" s="77">
+      <c r="AC252" s="141">
         <v>0.32224267899999998</v>
       </c>
-      <c r="AD252" s="77">
+      <c r="AD252" s="141">
         <v>0.36321352000000001</v>
       </c>
-      <c r="AE252" s="77">
+      <c r="AE252" s="141">
         <v>0.17882509799999999</v>
       </c>
-      <c r="AF252" s="77">
+      <c r="AF252" s="141">
         <v>0.29740473699999997</v>
       </c>
     </row>
@@ -28444,19 +28461,19 @@
       <c r="Z253" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AA253" s="77">
+      <c r="AA253" s="140">
         <v>1.7292100000000001E-4</v>
       </c>
       <c r="AB253" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AC253" s="77">
+      <c r="AC253" s="140">
         <v>1.312447E-3</v>
       </c>
       <c r="AD253" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AE253" s="77">
+      <c r="AE253" s="140">
         <v>1.4188950000000001E-3</v>
       </c>
       <c r="AF253" s="77" t="s">
@@ -28542,19 +28559,19 @@
       <c r="Z254" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AA254" s="77">
+      <c r="AA254" s="141">
         <v>0.125678176</v>
       </c>
       <c r="AB254" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AC254" s="77">
+      <c r="AC254" s="141">
         <v>0.27134870999999999</v>
       </c>
       <c r="AD254" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AE254" s="77">
+      <c r="AE254" s="141">
         <v>0.32495359699999998</v>
       </c>
       <c r="AF254" s="77" t="s">
@@ -28660,33 +28677,872 @@
       </c>
     </row>
     <row r="256" spans="1:32">
-      <c r="A256" t="s">
+      <c r="A256" s="123" t="s">
         <v>289</v>
       </c>
+      <c r="B256" s="123">
+        <v>0.79619742911153124</v>
+      </c>
+      <c r="C256" s="123">
+        <v>0.819581</v>
+      </c>
+      <c r="D256" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="E256" s="123">
+        <v>0.71907848771266536</v>
+      </c>
+      <c r="F256" s="123">
+        <v>0.80606450000000007</v>
+      </c>
+      <c r="G256" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="H256" s="123">
+        <v>3.8889060680529304</v>
+      </c>
+      <c r="I256" s="123">
+        <v>4.6842420000000002</v>
+      </c>
+      <c r="J256" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="K256" s="123">
+        <v>40</v>
+      </c>
+      <c r="L256" s="123">
+        <v>0</v>
+      </c>
+      <c r="M256" s="124">
+        <v>0</v>
+      </c>
+      <c r="N256" s="123">
+        <v>31</v>
+      </c>
+      <c r="O256" s="124">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="P256" s="124">
+        <v>0.10064935064935066</v>
+      </c>
+      <c r="Q256" s="123" t="s">
+        <v>296</v>
+      </c>
+      <c r="R256" s="123">
+        <v>5.1205979423698644E-2</v>
+      </c>
+      <c r="S256" s="123">
+        <v>4.4417765691218636E-2</v>
+      </c>
+      <c r="T256" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="U256" s="123">
+        <v>0.21672505593039848</v>
+      </c>
+      <c r="V256" s="123">
+        <v>0.16747213436792999</v>
+      </c>
+      <c r="W256" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="X256" s="123">
+        <v>1.983584323376935</v>
+      </c>
+      <c r="Y256" s="123">
+        <v>2.019214799372766</v>
+      </c>
+      <c r="Z256" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA256" s="126">
+        <v>1.46654978564403E-3</v>
+      </c>
+      <c r="AB256" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC256" s="126">
+        <v>1.8172297561323701E-3</v>
+      </c>
+      <c r="AD256" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE256" s="126">
+        <v>1.0509840262619899E-2</v>
+      </c>
+      <c r="AF256" s="123" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="257" spans="1:1">
-      <c r="A257" t="s">
+    <row r="257" spans="1:32">
+      <c r="A257" s="77" t="s">
         <v>290</v>
       </c>
+      <c r="B257" s="77">
+        <v>0.79323983200000003</v>
+      </c>
+      <c r="C257" s="77">
+        <v>0.79738500000000001</v>
+      </c>
+      <c r="D257" s="77">
+        <v>0.85350999999999999</v>
+      </c>
+      <c r="E257" s="77">
+        <v>0.73326657399999995</v>
+      </c>
+      <c r="F257" s="77">
+        <v>0.78954250000000004</v>
+      </c>
+      <c r="G257" s="77">
+        <v>0.87688500000000003</v>
+      </c>
+      <c r="H257" s="77">
+        <v>3.9319952329999999</v>
+      </c>
+      <c r="I257" s="77">
+        <v>3.0966</v>
+      </c>
+      <c r="J257" s="77">
+        <v>5.8177500000000002</v>
+      </c>
+      <c r="K257" s="77">
+        <v>6</v>
+      </c>
+      <c r="L257" s="77">
+        <v>2</v>
+      </c>
+      <c r="M257" s="80">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="N257" s="77">
+        <v>3</v>
+      </c>
+      <c r="O257" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="P257" s="80">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="Q257" s="77" t="s">
+        <v>296</v>
+      </c>
+      <c r="R257" s="77">
+        <v>6.3205911000000004E-2</v>
+      </c>
+      <c r="S257" s="77">
+        <v>4.3532581000000001E-2</v>
+      </c>
+      <c r="T257" s="77">
+        <v>8.4200000000000004E-3</v>
+      </c>
+      <c r="U257" s="77">
+        <v>0.22820193499999999</v>
+      </c>
+      <c r="V257" s="77">
+        <v>0.25437464399999998</v>
+      </c>
+      <c r="W257" s="77">
+        <v>1.9785000000000001E-2</v>
+      </c>
+      <c r="X257" s="77">
+        <v>1.9672635119999999</v>
+      </c>
+      <c r="Y257" s="77">
+        <v>2.729567898</v>
+      </c>
+      <c r="Z257" s="77">
+        <v>0.16470000000000001</v>
+      </c>
+      <c r="AA257" s="141">
+        <v>0.431091803</v>
+      </c>
+      <c r="AB257" s="141">
+        <v>0.121685168</v>
+      </c>
+      <c r="AC257" s="141">
+        <v>0.34448269599999998</v>
+      </c>
+      <c r="AD257" s="141">
+        <v>0.30934616700000001</v>
+      </c>
+      <c r="AE257" s="141">
+        <v>0.292211316</v>
+      </c>
+      <c r="AF257" s="141">
+        <v>0.14844049300000001</v>
+      </c>
     </row>
-    <row r="258" spans="1:1">
-      <c r="A258" t="s">
+    <row r="258" spans="1:32">
+      <c r="A258" s="123" t="s">
         <v>291</v>
       </c>
+      <c r="B258" s="123">
+        <v>0.77375819819819824</v>
+      </c>
+      <c r="C258" s="123">
+        <v>0.83098000000000005</v>
+      </c>
+      <c r="D258" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="E258" s="123">
+        <v>0.69708576576576564</v>
+      </c>
+      <c r="F258" s="123">
+        <v>0.83123999999999998</v>
+      </c>
+      <c r="G258" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="H258" s="123">
+        <v>3.4619285585585584</v>
+      </c>
+      <c r="I258" s="123">
+        <v>5.9494100000000003</v>
+      </c>
+      <c r="J258" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="K258" s="123">
+        <v>2</v>
+      </c>
+      <c r="L258" s="123">
+        <v>0</v>
+      </c>
+      <c r="M258" s="124">
+        <v>0</v>
+      </c>
+      <c r="N258" s="123">
+        <v>2</v>
+      </c>
+      <c r="O258" s="124">
+        <v>1</v>
+      </c>
+      <c r="P258" s="124">
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="Q258" s="123" t="s">
+        <v>300</v>
+      </c>
+      <c r="R258" s="123">
+        <v>6.0803573748072527E-2</v>
+      </c>
+      <c r="S258" s="123">
+        <v>3.014E-2</v>
+      </c>
+      <c r="T258" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="U258" s="123">
+        <v>0.20657011437364681</v>
+      </c>
+      <c r="V258" s="123">
+        <v>3.3420000000000005E-2</v>
+      </c>
+      <c r="W258" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="X258" s="123">
+        <v>1.8630769688852671</v>
+      </c>
+      <c r="Y258" s="123">
+        <v>1.2457699999999998</v>
+      </c>
+      <c r="Z258" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA258" s="125">
+        <v>0.117220897622846</v>
+      </c>
+      <c r="AB258" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC258" s="125">
+        <v>7.1623435093714799E-2</v>
+      </c>
+      <c r="AD258" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE258" s="125">
+        <v>0.110330451248231</v>
+      </c>
+      <c r="AF258" s="123" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="259" spans="1:1">
-      <c r="A259" t="s">
+    <row r="259" spans="1:32">
+      <c r="A259" s="123" t="s">
         <v>292</v>
       </c>
+      <c r="B259" s="123">
+        <v>0.68999636079249216</v>
+      </c>
+      <c r="C259" s="123">
+        <v>0.7348433333333334</v>
+      </c>
+      <c r="D259" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="E259" s="123">
+        <v>0.53780417101147027</v>
+      </c>
+      <c r="F259" s="123">
+        <v>0.73664333333333332</v>
+      </c>
+      <c r="G259" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="H259" s="123">
+        <v>2.6296687799791449</v>
+      </c>
+      <c r="I259" s="123">
+        <v>4.3210266666666666</v>
+      </c>
+      <c r="J259" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="K259" s="123">
+        <v>3</v>
+      </c>
+      <c r="L259" s="123">
+        <v>0</v>
+      </c>
+      <c r="M259" s="124">
+        <v>0</v>
+      </c>
+      <c r="N259" s="123">
+        <v>2</v>
+      </c>
+      <c r="O259" s="124">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="P259" s="124">
+        <v>7.575757575757576E-3</v>
+      </c>
+      <c r="Q259" s="123" t="s">
+        <v>300</v>
+      </c>
+      <c r="R259" s="123">
+        <v>0.14040718229655466</v>
+      </c>
+      <c r="S259" s="123">
+        <v>0.13747583698801605</v>
+      </c>
+      <c r="T259" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="U259" s="123">
+        <v>0.25361473497033438</v>
+      </c>
+      <c r="V259" s="123">
+        <v>0.29251618420563025</v>
+      </c>
+      <c r="W259" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="X259" s="123">
+        <v>1.8654525380271629</v>
+      </c>
+      <c r="Y259" s="123">
+        <v>0.94558119469221447</v>
+      </c>
+      <c r="Z259" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA259" s="125">
+        <v>0.31475215426963898</v>
+      </c>
+      <c r="AB259" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC259" s="125">
+        <v>0.180312916610746</v>
+      </c>
+      <c r="AD259" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE259" s="126">
+        <v>4.5624813453455301E-2</v>
+      </c>
+      <c r="AF259" s="123" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="260" spans="1:1">
-      <c r="A260" t="s">
+    <row r="260" spans="1:32">
+      <c r="A260" s="77" t="s">
         <v>293</v>
       </c>
+      <c r="B260" s="77">
+        <v>0.70865364200000003</v>
+      </c>
+      <c r="C260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="D260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="E260" s="77">
+        <v>0.54949085499999994</v>
+      </c>
+      <c r="F260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="G260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="H260" s="77">
+        <v>2.492049723</v>
+      </c>
+      <c r="I260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="J260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="K260" s="77">
+        <v>0</v>
+      </c>
+      <c r="L260" s="77">
+        <v>0</v>
+      </c>
+      <c r="M260" s="80">
+        <v>0</v>
+      </c>
+      <c r="N260" s="77">
+        <v>0</v>
+      </c>
+      <c r="O260" s="80">
+        <v>0</v>
+      </c>
+      <c r="P260" s="80">
+        <v>0</v>
+      </c>
+      <c r="Q260" s="77" t="s">
+        <v>300</v>
+      </c>
+      <c r="R260" s="77">
+        <v>0.110718541</v>
+      </c>
+      <c r="S260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="T260" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="U260" s="77">
+        <v>0.239751249</v>
+      </c>
+      <c r="V260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="W260" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="X260" s="77">
+        <v>2.0153830899999998</v>
+      </c>
+      <c r="Y260" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z260" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA260" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB260" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC260" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD260" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE260" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF260" s="77" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="261" spans="1:1">
-      <c r="A261" t="s">
+    <row r="261" spans="1:32">
+      <c r="A261" s="123" t="s">
         <v>294</v>
+      </c>
+      <c r="B261" s="123">
+        <v>0.66720381052631594</v>
+      </c>
+      <c r="C261" s="123">
+        <v>0.78712599999999999</v>
+      </c>
+      <c r="D261" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="E261" s="123">
+        <v>0.53801955789473688</v>
+      </c>
+      <c r="F261" s="123">
+        <v>0.75298399999999999</v>
+      </c>
+      <c r="G261" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="H261" s="123">
+        <v>2.2182053473684209</v>
+      </c>
+      <c r="I261" s="123">
+        <v>4.3897599999999999</v>
+      </c>
+      <c r="J261" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="K261" s="123">
+        <v>5</v>
+      </c>
+      <c r="L261" s="123">
+        <v>0</v>
+      </c>
+      <c r="M261" s="124">
+        <v>0</v>
+      </c>
+      <c r="N261" s="123">
+        <v>4</v>
+      </c>
+      <c r="O261" s="124">
+        <v>0.8</v>
+      </c>
+      <c r="P261" s="124">
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="Q261" s="123" t="s">
+        <v>34</v>
+      </c>
+      <c r="R261" s="123">
+        <v>0.11917524481025896</v>
+      </c>
+      <c r="S261" s="123">
+        <v>3.1242760825509631E-2</v>
+      </c>
+      <c r="T261" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="U261" s="123">
+        <v>0.21496740908140696</v>
+      </c>
+      <c r="V261" s="123">
+        <v>9.7747814829795526E-2</v>
+      </c>
+      <c r="W261" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="X261" s="123">
+        <v>1.6960750644674449</v>
+      </c>
+      <c r="Y261" s="123">
+        <v>1.6246410944328595</v>
+      </c>
+      <c r="Z261" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA261" s="126">
+        <v>6.6427076803390395E-4</v>
+      </c>
+      <c r="AB261" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC261" s="126">
+        <v>4.3338396908630498E-3</v>
+      </c>
+      <c r="AD261" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE261" s="126">
+        <v>2.0535242208296101E-2</v>
+      </c>
+      <c r="AF261" s="123" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="262" spans="1:32">
+      <c r="A262" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B262" s="1">
+        <f>AVERAGE(B2:B261)</f>
+        <v>0.72557881651433609</v>
+      </c>
+      <c r="C262" s="1">
+        <f t="shared" ref="C262:AF262" si="1">AVERAGE(C2:C261)</f>
+        <v>0.76646218719017056</v>
+      </c>
+      <c r="D262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67422784967307492</v>
+      </c>
+      <c r="E262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.58443663797369305</v>
+      </c>
+      <c r="F262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.68580681532260013</v>
+      </c>
+      <c r="G262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45041343123829225</v>
+      </c>
+      <c r="H262" s="1">
+        <f t="shared" si="1"/>
+        <v>2.598308001595437</v>
+      </c>
+      <c r="I262" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5019988309849031</v>
+      </c>
+      <c r="J262" s="1">
+        <f t="shared" si="1"/>
+        <v>1.586315496487529</v>
+      </c>
+      <c r="K262" s="1">
+        <f t="shared" si="1"/>
+        <v>11.594594594594595</v>
+      </c>
+      <c r="L262" s="1">
+        <f t="shared" si="1"/>
+        <v>2.0386100386100385</v>
+      </c>
+      <c r="M262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.19056938173384649</v>
+      </c>
+      <c r="N262" s="1">
+        <f t="shared" si="1"/>
+        <v>5.24609375</v>
+      </c>
+      <c r="O262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.37899423635829493</v>
+      </c>
+      <c r="P262" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3657966545198675E-2</v>
+      </c>
+      <c r="Q262" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.11283593767434612</v>
+      </c>
+      <c r="S262" s="1">
+        <f t="shared" si="1"/>
+        <v>5.94069127016396E-2</v>
+      </c>
+      <c r="T262" s="1">
+        <f t="shared" si="1"/>
+        <v>6.6561098343756717E-2</v>
+      </c>
+      <c r="U262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.22574983660441691</v>
+      </c>
+      <c r="V262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14848493104811569</v>
+      </c>
+      <c r="W262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10466684174292902</v>
+      </c>
+      <c r="X262" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7966777962846503</v>
+      </c>
+      <c r="Y262" s="1">
+        <f t="shared" si="1"/>
+        <v>1.250642888386744</v>
+      </c>
+      <c r="Z262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.84146243938981147</v>
+      </c>
+      <c r="AA262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.11929791255377606</v>
+      </c>
+      <c r="AB262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.15174987162499823</v>
+      </c>
+      <c r="AC262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13149233008052322</v>
+      </c>
+      <c r="AD262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13633531528276352</v>
+      </c>
+      <c r="AE262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.12462687396115429</v>
+      </c>
+      <c r="AF262" s="1">
+        <f t="shared" si="1"/>
+        <v>0.12101555956435316</v>
+      </c>
+    </row>
+    <row r="263" spans="1:32">
+      <c r="A263" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B263" s="1">
+        <f>STDEV(B2:B261)</f>
+        <v>0.12375695767753941</v>
+      </c>
+      <c r="C263" s="1">
+        <f t="shared" ref="C263:AF263" si="2">STDEV(C2:C261)</f>
+        <v>0.22867425328076113</v>
+      </c>
+      <c r="D263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.19905797425063318</v>
+      </c>
+      <c r="E263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.12778919047588613</v>
+      </c>
+      <c r="F263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.16049106815573827</v>
+      </c>
+      <c r="G263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.19083822761026387</v>
+      </c>
+      <c r="H263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.88025416078482421</v>
+      </c>
+      <c r="I263" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2637220561955194</v>
+      </c>
+      <c r="J263" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5422927196379068</v>
+      </c>
+      <c r="K263" s="1">
+        <f t="shared" si="2"/>
+        <v>14.250857778131421</v>
+      </c>
+      <c r="L263" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4504318905119149</v>
+      </c>
+      <c r="M263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.23431334596738801</v>
+      </c>
+      <c r="N263" s="1">
+        <f t="shared" si="2"/>
+        <v>7.739254687161103</v>
+      </c>
+      <c r="O263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.29543388988801739</v>
+      </c>
+      <c r="P263" s="1">
+        <f t="shared" si="2"/>
+        <v>4.9938145714456095E-2</v>
+      </c>
+      <c r="Q263" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.18510862495664354</v>
+      </c>
+      <c r="S263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.11423600030743716</v>
+      </c>
+      <c r="T263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.25908590748415944</v>
+      </c>
+      <c r="U263" s="1">
+        <f t="shared" si="2"/>
+        <v>9.3810024500728589E-2</v>
+      </c>
+      <c r="V263" s="1">
+        <f t="shared" si="2"/>
+        <v>8.5366996763570124E-2</v>
+      </c>
+      <c r="W263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10853152834318112</v>
+      </c>
+      <c r="X263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.25090046441287772</v>
+      </c>
+      <c r="Y263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.73370740526566891</v>
+      </c>
+      <c r="Z263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.84791261171239973</v>
+      </c>
+      <c r="AA263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.14589556787145413</v>
+      </c>
+      <c r="AB263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.12835707819651607</v>
+      </c>
+      <c r="AC263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.14939215511569179</v>
+      </c>
+      <c r="AD263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.12587018044824161</v>
+      </c>
+      <c r="AE263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.14022799455519522</v>
+      </c>
+      <c r="AF263" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10545895000018869</v>
+      </c>
+    </row>
+    <row r="264" spans="1:32">
+      <c r="Z264" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AA264" s="142">
+        <v>7.776982E-3</v>
+      </c>
+      <c r="AB264" s="143">
+        <v>1.7342689999999998E-5</v>
+      </c>
+      <c r="AC264" s="143">
+        <v>1.6822650000000001E-13</v>
+      </c>
+      <c r="AD264" s="143">
+        <v>1.050539E-26</v>
+      </c>
+      <c r="AE264" s="143">
+        <v>1.5451570000000001E-17</v>
+      </c>
+      <c r="AF264" s="143">
+        <v>2.9771060000000001E-27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>